<commit_message>
Added Excel template loader for Outlook automation
</commit_message>
<xml_diff>
--- a/program/outlookmail_送付フォーマット.xlsx
+++ b/program/outlookmail_送付フォーマット.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\□LMC□本社⑧\Desktop\python_program\airwork-project\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85387EE0-2F4E-4C4D-AECB-818C5E5A346C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CCEA2-A38D-480C-AFC4-5AEE1BDAF324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8298409F-DE15-4F54-BF04-6F50FA9F6479}"/>
   </bookViews>
   <sheets>
     <sheet name="応募者共有先リスト" sheetId="1" r:id="rId1"/>
-    <sheet name="処理完了の通知先" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -75,39 +74,6 @@
     <t>担当者</t>
     <rPh sb="0" eb="3">
       <t>タントウシャ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>氏名</t>
-    <rPh sb="0" eb="2">
-      <t>シメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>本日の自動振分け処理完了しました。</t>
-    <rPh sb="0" eb="2">
-      <t>ホンジツ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フリワ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アドレス（宛先）</t>
-    <rPh sb="5" eb="7">
-      <t>アテサキ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -145,29 +111,6 @@
     <t>山田　太郎</t>
     <rPh sb="0" eb="2">
       <t>ヤマダ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>タロウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>応募者の共有が完了しました</t>
-    <rPh sb="0" eb="3">
-      <t>オウボシャ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>キョウユウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>田中　太郎</t>
-    <rPh sb="0" eb="2">
-      <t>タナカ</t>
     </rPh>
     <rPh sb="3" eb="5">
       <t>タロウ</t>
@@ -325,7 +268,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -360,9 +303,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -846,7 +786,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -882,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -891,10 +831,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -902,8 +842,8 @@
       <c r="G2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>10</v>
+      <c r="H2" s="13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -916,62 +856,62 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H5" s="13"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H6" s="13"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H7" s="13"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H8" s="13"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H9" s="13"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H10" s="13"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H11" s="13"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H12" s="13"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H13" s="13"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H14" s="13"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H15" s="13"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H16" s="13"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H17" s="13"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H18" s="13"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H19" s="13"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H20" s="13"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H21" s="13"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
@@ -982,51 +922,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768295AC-5578-42B2-9613-C822E6056208}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.8984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="D2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>